<commit_message>
cleaning script and data for manuscript submission
</commit_message>
<xml_diff>
--- a/Data/Food/food_production/feed_ratios.xlsx
+++ b/Data/Food/food_production/feed_ratios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/sibeal_mccourt_mail_mcgill_ca/Documents/R/Canadian_N_Footprint/Data/Food/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/sibeal_mccourt_mail_mcgill_ca/Documents/R/Canadian_N_Footprint/Data/Food/food_production/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="11_B9DE4158B272683391325315491AECD6AA688E4A" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F2F71FB0-60AD-468C-BC6A-1850618B1FD5}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="11_B9DE4158B272683391325315491AECD6AA688E4A" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{922B9C37-9545-401D-B554-92B5AE5773D2}"/>
   <bookViews>
-    <workbookView xWindow="3795" yWindow="105" windowWidth="23475" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13095" yWindow="570" windowWidth="17115" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -442,7 +442,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,8 +690,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <f>(7900+3800)/2</f>
-        <v>5850</v>
+        <v>7900</v>
       </c>
       <c r="C9">
         <v>0.1</v>

</xml_diff>